<commit_message>
Make the initial guess an array as expected.
</commit_message>
<xml_diff>
--- a/src/dataframes/input/output_portfolio.xlsx
+++ b/src/dataframes/input/output_portfolio.xlsx
@@ -488,19 +488,19 @@
         <v>606.9299999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003232190670004752</v>
+        <v>0.003130648843205768</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01852009565666453</v>
+        <v>0.01850765251460834</v>
       </c>
       <c r="F2" t="n">
         <v>0.01401156838006895</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="H2" t="n">
-        <v>24257.16</v>
+        <v>22091.34</v>
       </c>
     </row>
     <row r="3">
@@ -516,10 +516,10 @@
         <v>567.7</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001301916575971996</v>
+        <v>0.001316074188654831</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01590762040556708</v>
+        <v>0.01585281793820317</v>
       </c>
       <c r="F3" t="n">
         <v>0.0131059057376718</v>
@@ -544,10 +544,10 @@
         <v>617.34</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001263900035922273</v>
+        <v>0.001184645926661158</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02235761583913525</v>
+        <v>0.02227509086647682</v>
       </c>
       <c r="F4" t="n">
         <v>0.01425189333819678</v>
@@ -572,10 +572,10 @@
         <v>214.8</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0007478559693877101</v>
+        <v>0.001043213982647104</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02030180036667387</v>
+        <v>0.02021608906402109</v>
       </c>
       <c r="F5" t="n">
         <v>0.004958866571167699</v>
@@ -600,10 +600,10 @@
         <v>418.56</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00220281227972601</v>
+        <v>0.002176021606322795</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02348137052817831</v>
+        <v>0.02342341165530148</v>
       </c>
       <c r="F6" t="n">
         <v>0.0096628640224765</v>
@@ -628,19 +628,19 @@
         <v>891.98</v>
       </c>
       <c r="D7" t="n">
-        <v>0.004228891655386579</v>
+        <v>0.004115310161708273</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04931837619874675</v>
+        <v>0.04909455604170841</v>
       </c>
       <c r="F7" t="n">
         <v>0.02059222441410691</v>
       </c>
       <c r="G7" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="H7" t="n">
-        <v>1299.49</v>
+        <v>433.16</v>
       </c>
     </row>
     <row r="8">
@@ -656,10 +656,10 @@
         <v>3451.95</v>
       </c>
       <c r="D8" t="n">
-        <v>-8.44719358350961e-06</v>
+        <v>6.118006989292327e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01798167549163614</v>
+        <v>0.01791952477032176</v>
       </c>
       <c r="F8" t="n">
         <v>0.07969161759935912</v>
@@ -684,19 +684,19 @@
         <v>4986.22</v>
       </c>
       <c r="D9" t="n">
-        <v>0.004304360854708853</v>
+        <v>0.005117839680748134</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0415393425607061</v>
+        <v>0.04199428619745113</v>
       </c>
       <c r="F9" t="n">
         <v>0.1151117303281555</v>
       </c>
       <c r="G9" t="n">
-        <v>0.02</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>866.33</v>
+        <v>3032.14</v>
       </c>
     </row>
     <row r="10">
@@ -712,10 +712,10 @@
         <v>5934.47</v>
       </c>
       <c r="D10" t="n">
-        <v>0.009372878905365301</v>
+        <v>0.01008735305826615</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06710373376196115</v>
+        <v>0.06709706348823545</v>
       </c>
       <c r="F10" t="n">
         <v>0.1370030023305288</v>
@@ -740,19 +740,19 @@
         <v>25626.4</v>
       </c>
       <c r="D11" t="n">
-        <v>0.003569208492126451</v>
+        <v>0.00362844919629976</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02792153929624141</v>
+        <v>0.02775403592979557</v>
       </c>
       <c r="F11" t="n">
         <v>0.5916103272782679</v>
       </c>
       <c r="G11" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="H11" t="n">
-        <v>10829.09</v>
+        <v>11695.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update requirements. New run outputs.
</commit_message>
<xml_diff>
--- a/src/dataframes/input/output_portfolio.xlsx
+++ b/src/dataframes/input/output_portfolio.xlsx
@@ -488,19 +488,19 @@
         <v>606.9299999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003130648843205768</v>
+        <v>0.003173959397873089</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01850765251460834</v>
+        <v>0.01857558657652227</v>
       </c>
       <c r="F2" t="n">
         <v>0.01401156838006895</v>
       </c>
       <c r="G2" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="H2" t="n">
-        <v>22091.34</v>
+        <v>21658.18</v>
       </c>
     </row>
     <row r="3">
@@ -516,10 +516,10 @@
         <v>567.7</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001316074188654831</v>
+        <v>0.001358097442220604</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01585281793820317</v>
+        <v>0.01592194719999851</v>
       </c>
       <c r="F3" t="n">
         <v>0.0131059057376718</v>
@@ -544,10 +544,10 @@
         <v>617.34</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001184645926661158</v>
+        <v>0.001279591134608583</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02227509086647682</v>
+        <v>0.02234653965257309</v>
       </c>
       <c r="F4" t="n">
         <v>0.01425189333819678</v>
@@ -572,10 +572,10 @@
         <v>214.8</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001043213982647104</v>
+        <v>0.0009345652867390518</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02021608906402109</v>
+        <v>0.02036751953979167</v>
       </c>
       <c r="F5" t="n">
         <v>0.004958866571167699</v>
@@ -600,10 +600,10 @@
         <v>418.56</v>
       </c>
       <c r="D6" t="n">
-        <v>0.002176021606322795</v>
+        <v>0.0021229050052257</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02342341165530148</v>
+        <v>0.02360997313468402</v>
       </c>
       <c r="F6" t="n">
         <v>0.0096628640224765</v>
@@ -628,19 +628,19 @@
         <v>891.98</v>
       </c>
       <c r="D7" t="n">
-        <v>0.004115310161708273</v>
+        <v>0.003779962272645701</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04909455604170841</v>
+        <v>0.0492683155047368</v>
       </c>
       <c r="F7" t="n">
         <v>0.02059222441410691</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>433.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -656,10 +656,10 @@
         <v>3451.95</v>
       </c>
       <c r="D8" t="n">
-        <v>6.118006989292327e-05</v>
+        <v>0.0001458607358971155</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01791952477032176</v>
+        <v>0.01794364018502862</v>
       </c>
       <c r="F8" t="n">
         <v>0.07969161759935912</v>
@@ -684,19 +684,19 @@
         <v>4986.22</v>
       </c>
       <c r="D9" t="n">
-        <v>0.005117839680748134</v>
+        <v>0.004854294480505244</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04199428619745113</v>
+        <v>0.0423008279237936</v>
       </c>
       <c r="F9" t="n">
         <v>0.1151117303281555</v>
       </c>
       <c r="G9" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="H9" t="n">
-        <v>3032.14</v>
+        <v>2598.98</v>
       </c>
     </row>
     <row r="10">
@@ -712,19 +712,19 @@
         <v>5934.47</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01008735305826615</v>
+        <v>0.009271276528460179</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06709706348823545</v>
+        <v>0.06758358167121899</v>
       </c>
       <c r="F10" t="n">
         <v>0.1370030023305288</v>
       </c>
       <c r="G10" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="H10" t="n">
-        <v>6064.29</v>
+        <v>5631.13</v>
       </c>
     </row>
     <row r="11">
@@ -740,19 +740,19 @@
         <v>25626.4</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00362844919629976</v>
+        <v>0.004078503750362078</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02775403592979557</v>
+        <v>0.02793348604957986</v>
       </c>
       <c r="F11" t="n">
         <v>0.5916103272782679</v>
       </c>
       <c r="G11" t="n">
-        <v>0.27</v>
+        <v>0.31</v>
       </c>
       <c r="H11" t="n">
-        <v>11695.41</v>
+        <v>13428.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>